<commit_message>
coding being vs becoming
</commit_message>
<xml_diff>
--- a/data/website/walkaway testimonials.xlsx
+++ b/data/website/walkaway testimonials.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="110">
   <si>
     <t>Title</t>
   </si>
@@ -342,6 +342,21 @@
   </si>
   <si>
     <t>1,842 views</t>
+  </si>
+  <si>
+    <t>Being</t>
+  </si>
+  <si>
+    <t>Becoming</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -398,12 +413,18 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -418,15 +439,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,411 +735,636 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="106.6640625" customWidth="1"/>
+    <col min="2" max="2" width="145.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="212" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="101" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="166" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A6" s="4" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="229" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="70" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="166" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="150" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="409.6" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A12" s="4" t="s">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="229" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="181" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A14" s="4" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="101" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="262" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A16" s="4" t="s">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="142" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="118" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A18" s="4" t="s">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="197" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="188" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A20" s="4" t="s">
+      <c r="D19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="133" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="86" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="150" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A23" s="4" t="s">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="409.6" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A24" s="4" t="s">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="373" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="246" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="181" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="230" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="198" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="102" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A30" s="4" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="197" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="70" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D31" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="310" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="118" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="134" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="49" x14ac:dyDescent="0.45">
-      <c r="A35" s="4" t="s">
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="49" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="50" x14ac:dyDescent="0.5">
+      <c r="D35" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="5" t="s">
         <v>104</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>